<commit_message>
Reverted program to produce separate excel files
</commit_message>
<xml_diff>
--- a/combined_tables.xlsx
+++ b/combined_tables.xlsx
@@ -61,7 +61,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>ffxqa</t>
+    <t>open</t>
   </si>
   <si>
     <t>resolved</t>
@@ -109,10 +109,10 @@
     <t>Total # Tickets</t>
   </si>
   <si>
+    <t>Customer Generated Ticket</t>
+  </si>
+  <si>
     <t>Customer Testing</t>
-  </si>
-  <si>
-    <t>FFX Testing</t>
   </si>
   <si>
     <t>Meeting To Be Scheduled</t>
@@ -518,7 +518,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -534,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -569,16 +569,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
       </c>
       <c r="F8" s="3">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -609,16 +609,16 @@
         <v>5</v>
       </c>
       <c r="C10" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
       </c>
       <c r="F10" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -629,16 +629,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -664,13 +664,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -681,16 +681,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D17" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="4">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -732,16 +732,16 @@
         <v>13</v>
       </c>
       <c r="B20" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
         <v>3</v>
       </c>
       <c r="E20" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -773,10 +773,10 @@
         <v>0</v>
       </c>
       <c r="C25" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -793,16 +793,16 @@
         <v>0</v>
       </c>
       <c r="C26" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D26" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E26" s="4">
         <v>0</v>
       </c>
       <c r="F26" s="4">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -853,16 +853,16 @@
         <v>8</v>
       </c>
       <c r="C29" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
       </c>
       <c r="F29" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -888,16 +888,16 @@
         <v>10</v>
       </c>
       <c r="B35" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C35" s="3">
+        <v>0</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1</v>
+      </c>
+      <c r="E35" s="3">
         <v>3</v>
-      </c>
-      <c r="D35" s="3">
-        <v>2</v>
-      </c>
-      <c r="E35" s="3">
-        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -905,13 +905,13 @@
         <v>11</v>
       </c>
       <c r="B36" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" s="4">
         <v>2</v>
       </c>
       <c r="D36" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="4">
         <v>5</v>
@@ -925,13 +925,13 @@
         <v>2</v>
       </c>
       <c r="C37" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" s="3">
         <v>1</v>
       </c>
       <c r="E37" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -939,16 +939,16 @@
         <v>13</v>
       </c>
       <c r="B38" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C38" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1">
         <v>3</v>
       </c>
       <c r="E38" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -975,16 +975,16 @@
         <v>22</v>
       </c>
       <c r="B43" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
       </c>
       <c r="D43" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E43" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -992,16 +992,16 @@
         <v>23</v>
       </c>
       <c r="B44" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C44" s="4">
         <v>0</v>
       </c>
       <c r="D44" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E44" s="4">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1026,16 +1026,16 @@
         <v>13</v>
       </c>
       <c r="B46" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46" s="1">
         <v>1</v>
       </c>
       <c r="D46" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E46" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -1064,7 +1064,7 @@
         <v>26</v>
       </c>
       <c r="B51" s="4">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1072,7 +1072,7 @@
         <v>13</v>
       </c>
       <c r="B52" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -1096,7 +1096,7 @@
         <v>10</v>
       </c>
       <c r="B57" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1104,7 +1104,7 @@
         <v>11</v>
       </c>
       <c r="B58" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1120,7 +1120,7 @@
         <v>13</v>
       </c>
       <c r="B60" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -1144,7 +1144,7 @@
         <v>10</v>
       </c>
       <c r="B64" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1160,7 +1160,7 @@
         <v>12</v>
       </c>
       <c r="B66" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1168,7 +1168,7 @@
         <v>13</v>
       </c>
       <c r="B67" s="1">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>

</xml_diff>

<commit_message>
Merging all workbooks into individual spreadsheets of a single master workbook
</commit_message>
<xml_diff>
--- a/combined_tables.xlsx
+++ b/combined_tables.xlsx
@@ -518,7 +518,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -534,7 +534,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>

</xml_diff>